<commit_message>
KRST-82, Feature, Export Student List Info
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/学生信息批量导出模板.xlsx
+++ b/src/main/resources/templates/学生信息批量导出模板.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF4A33A-286B-45DA-B75D-842A0F5EBCFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB02EBF2-9963-402C-828D-3E85ECAD93EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="学生信息" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="辅助信息（请勿操作）" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>学生信息批量导出</t>
+  </si>
   <si>
     <t>学生编号</t>
   </si>
@@ -41,6 +44,9 @@
     <t>是否农历</t>
   </si>
   <si>
+    <t>年龄</t>
+  </si>
+  <si>
     <t>领洗日期</t>
   </si>
   <si>
@@ -80,10 +86,13 @@
     <t>负责员工</t>
   </si>
   <si>
-    <t>学生信息批量导出</t>
-  </si>
-  <si>
-    <t>年龄</t>
+    <t>校验码</t>
+  </si>
+  <si>
+    <t>H86D$8#a</t>
+  </si>
+  <si>
+    <t>日期格式</t>
   </si>
 </sst>
 </file>
@@ -91,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,6 +142,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -147,36 +165,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -459,11 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,100 +478,100 @@
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="2" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="5.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="6"/>
-    <col min="8" max="11" width="11.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="8" max="11" width="11.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17" style="5" customWidth="1"/>
     <col min="13" max="14" width="13.109375" customWidth="1"/>
-    <col min="15" max="15" width="35.21875" style="4" customWidth="1"/>
-    <col min="16" max="19" width="16.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="35.21875" style="5" customWidth="1"/>
+    <col min="16" max="19" width="16.33203125" style="5" customWidth="1"/>
     <col min="20" max="20" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -572,12 +579,12 @@
     <mergeCell ref="A1:T1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{3D86EBE7-EDC9-40CF-8B88-BEC639932D01}">
-      <formula1>"男,女"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M1048576 N3:N1048576" xr:uid="{E97CB795-5C1B-4960-9A0D-66354EC3E106}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:N1048576" xr:uid="{AC578309-DCC1-4508-87CA-1ADB70A95B10}">
       <formula1>8</formula1>
       <formula2>11</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{40D4D486-3D54-4018-85E3-AD8FE88C50DE}">
+      <formula1>"男,女"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -586,19 +593,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EF1920-FAD0-4FE4-8E04-18B5E64A99EF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E99165E-90FF-4BA8-854B-C9AFB361B01E}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44562</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KRST-82, Feature, Export Student List Info (#83)
* KRST-82, Feature, Export Student List Info

* ui change
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/学生信息批量导出模板.xlsx
+++ b/src/main/resources/templates/学生信息批量导出模板.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF4A33A-286B-45DA-B75D-842A0F5EBCFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB02EBF2-9963-402C-828D-3E85ECAD93EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="学生信息" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="辅助信息（请勿操作）" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>学生信息批量导出</t>
+  </si>
   <si>
     <t>学生编号</t>
   </si>
@@ -41,6 +44,9 @@
     <t>是否农历</t>
   </si>
   <si>
+    <t>年龄</t>
+  </si>
+  <si>
     <t>领洗日期</t>
   </si>
   <si>
@@ -80,10 +86,13 @@
     <t>负责员工</t>
   </si>
   <si>
-    <t>学生信息批量导出</t>
-  </si>
-  <si>
-    <t>年龄</t>
+    <t>校验码</t>
+  </si>
+  <si>
+    <t>H86D$8#a</t>
+  </si>
+  <si>
+    <t>日期格式</t>
   </si>
 </sst>
 </file>
@@ -91,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,6 +142,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -147,36 +165,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -459,11 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,100 +478,100 @@
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="2" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="5.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="6"/>
-    <col min="8" max="11" width="11.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="8" max="11" width="11.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17" style="5" customWidth="1"/>
     <col min="13" max="14" width="13.109375" customWidth="1"/>
-    <col min="15" max="15" width="35.21875" style="4" customWidth="1"/>
-    <col min="16" max="19" width="16.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="35.21875" style="5" customWidth="1"/>
+    <col min="16" max="19" width="16.33203125" style="5" customWidth="1"/>
     <col min="20" max="20" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -572,12 +579,12 @@
     <mergeCell ref="A1:T1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{3D86EBE7-EDC9-40CF-8B88-BEC639932D01}">
-      <formula1>"男,女"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M1048576 N3:N1048576" xr:uid="{E97CB795-5C1B-4960-9A0D-66354EC3E106}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:N1048576" xr:uid="{AC578309-DCC1-4508-87CA-1ADB70A95B10}">
       <formula1>8</formula1>
       <formula2>11</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{40D4D486-3D54-4018-85E3-AD8FE88C50DE}">
+      <formula1>"男,女"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -586,19 +593,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EF1920-FAD0-4FE4-8E04-18B5E64A99EF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E99165E-90FF-4BA8-854B-C9AFB361B01E}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44562</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>